<commit_message>
update der Bewertung der Use cases
</commit_message>
<xml_diff>
--- a/Hotelprojekt_vo da uebung/UseCase Bewertung.xlsx
+++ b/Hotelprojekt_vo da uebung/UseCase Bewertung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="15555"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -390,76 +389,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>42.916666666666671</c:v>
+                  <c:v>38.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.166666666666671</c:v>
+                  <c:v>40.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>38.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.833333333333329</c:v>
+                  <c:v>37.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.083333333333329</c:v>
+                  <c:v>35.416666666666671</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.666666666666664</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.083333333333336</c:v>
+                  <c:v>30.083333333333332</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.25</c:v>
+                  <c:v>28.916666666666668</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>25.749999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.416666666666668</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>25.916666666666664</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>25.583333333333336</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>25.083333333333332</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>24.833333333333332</c:v>
+                  <c:v>26.083333333333336</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24.75</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23.416666666666668</c:v>
+                  <c:v>22.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.916666666666668</c:v>
+                  <c:v>21.833333333333332</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.833333333333332</c:v>
+                  <c:v>21.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22.083333333333332</c:v>
+                  <c:v>20.583333333333332</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>21.166666666666668</c:v>
+                  <c:v>19.750000000000004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.75</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>18.666666666666668</c:v>
+                  <c:v>16.833333333333332</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>17.916666666666664</c:v>
+                  <c:v>18.916666666666664</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>17.333333333333332</c:v>
+                  <c:v>18.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>17.166666666666668</c:v>
+                  <c:v>16.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>16.666666666666668</c:v>
+                  <c:v>17.083333333333336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -474,11 +473,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="31936512"/>
-        <c:axId val="31938048"/>
+        <c:axId val="96024448"/>
+        <c:axId val="96025984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="31936512"/>
+        <c:axId val="96024448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,7 +486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="31938048"/>
+        <c:crossAx val="96025984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -495,7 +494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31938048"/>
+        <c:axId val="96025984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,13 +505,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="31936512"/>
+        <c:crossAx val="96024448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -654,7 +654,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>5.666666666666667</c:v>
+                  <c:v>4.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.5</c:v>
@@ -666,28 +666,28 @@
                   <c:v>5.833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.6666666666666661</c:v>
+                  <c:v>8.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.833333333333333</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>7.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.8333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>3.6666666666666665</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.8333333333333335</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5</c:v>
+                  <c:v>6.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.333333333333333</c:v>
+                  <c:v>4.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>3.8333333333333335</c:v>
@@ -702,7 +702,7 @@
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.166666666666667</c:v>
+                  <c:v>4.833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>5</c:v>
@@ -711,16 +711,16 @@
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5</c:v>
+                  <c:v>4.833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>2.3333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.833333333333333</c:v>
+                  <c:v>6.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6.166666666666667</c:v>
+                  <c:v>6.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>5.166666666666667</c:v>
@@ -738,11 +738,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="31962240"/>
-        <c:axId val="31963776"/>
+        <c:axId val="96070656"/>
+        <c:axId val="96072448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="31962240"/>
+        <c:axId val="96070656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +751,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="31963776"/>
+        <c:crossAx val="96072448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -759,7 +759,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31963776"/>
+        <c:axId val="96072448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="31962240"/>
+        <c:crossAx val="96070656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -807,6 +807,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -918,28 +919,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
+                  <c:v>8.6666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.8333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>7.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.333333333333333</c:v>
+                  <c:v>5.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.5</c:v>
+                  <c:v>6.833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.166666666666667</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.166666666666667</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>5.833333333333333</c:v>
@@ -951,43 +952,43 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.5</c:v>
+                  <c:v>3.8333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.666666666666667</c:v>
+                  <c:v>5.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1.6666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.666666666666667</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.333333333333333</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2</c:v>
+                  <c:v>1.6666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.6666666666666665</c:v>
+                  <c:v>3.6666666666666665</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2</c:v>
+                  <c:v>1.6666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>3.1666666666666665</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.8333333333333335</c:v>
+                  <c:v>4.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>2.3333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2</c:v>
+                  <c:v>2.3333333333333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1002,11 +1003,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="32516736"/>
-        <c:axId val="32530816"/>
+        <c:axId val="97796864"/>
+        <c:axId val="97798400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="32516736"/>
+        <c:axId val="97796864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1015,7 +1016,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="32530816"/>
+        <c:crossAx val="97798400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1023,7 +1024,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32530816"/>
+        <c:axId val="97798400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1034,13 +1035,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="32516736"/>
+        <c:crossAx val="97796864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1182,7 +1184,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>9.8333333333333339</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8.8333333333333339</c:v>
@@ -1191,7 +1193,7 @@
                   <c:v>7.833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.6666666666666661</c:v>
+                  <c:v>9.8333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7.666666666666667</c:v>
@@ -1209,49 +1211,49 @@
                   <c:v>5.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>6.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3.6666666666666665</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>7.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>7.666666666666667</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.333333333333333</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8.1666666666666661</c:v>
-                </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.5</c:v>
+                  <c:v>2.1666666666666665</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.666666666666667</c:v>
+                  <c:v>6.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.166666666666667</c:v>
+                  <c:v>4.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5</c:v>
+                  <c:v>4.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.5</c:v>
+                  <c:v>6.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>1.8333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.5</c:v>
+                  <c:v>2.8333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4</c:v>
+                  <c:v>3.8333333333333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1266,11 +1268,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="32555392"/>
-        <c:axId val="32556928"/>
+        <c:axId val="97835264"/>
+        <c:axId val="97837056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="32555392"/>
+        <c:axId val="97835264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1279,7 +1281,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="32556928"/>
+        <c:crossAx val="97837056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1287,7 +1289,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32556928"/>
+        <c:axId val="97837056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1298,7 +1300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="32555392"/>
+        <c:crossAx val="97835264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1531,11 +1533,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="47138688"/>
-        <c:axId val="47140224"/>
+        <c:axId val="97863552"/>
+        <c:axId val="97865088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47138688"/>
+        <c:axId val="97863552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1544,7 +1546,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47140224"/>
+        <c:crossAx val="97865088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1552,7 +1554,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47140224"/>
+        <c:axId val="97865088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1563,7 +1565,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47138688"/>
+        <c:crossAx val="97863552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2029,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2304,7 +2306,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="11">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D4" s="4">
         <v>8</v>
@@ -2316,28 +2318,28 @@
         <v>7</v>
       </c>
       <c r="G4" s="11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H4" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I4" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J4" s="11">
         <v>3</v>
       </c>
       <c r="K4" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4" s="4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="N4" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O4" s="11">
         <v>3</v>
@@ -2352,7 +2354,7 @@
         <v>2</v>
       </c>
       <c r="S4" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T4" s="11">
         <v>8</v>
@@ -2361,16 +2363,16 @@
         <v>7</v>
       </c>
       <c r="V4" s="11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W4" s="11">
         <v>3</v>
       </c>
       <c r="X4" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y4" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Z4" s="11">
         <v>6</v>
@@ -2774,28 +2776,28 @@
         <v>2</v>
       </c>
       <c r="C10" s="11">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11">
         <v>10</v>
       </c>
-      <c r="D10" s="11">
+      <c r="E10" s="11">
+        <v>8</v>
+      </c>
+      <c r="F10" s="11">
+        <v>10</v>
+      </c>
+      <c r="G10" s="11">
         <v>9</v>
       </c>
-      <c r="E10" s="11">
-        <v>8</v>
-      </c>
-      <c r="F10" s="11">
-        <v>8</v>
-      </c>
-      <c r="G10" s="11">
-        <v>7</v>
-      </c>
       <c r="H10" s="11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I10" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10" s="11">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K10" s="11">
         <v>5</v>
@@ -2807,43 +2809,43 @@
         <v>7</v>
       </c>
       <c r="N10" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O10" s="11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P10" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R10" s="11">
         <v>2</v>
       </c>
       <c r="S10" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T10" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U10" s="11">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="V10" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W10" s="11">
         <v>4</v>
       </c>
       <c r="X10" s="11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y10" s="11">
         <v>4</v>
       </c>
       <c r="Z10" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3244,7 +3246,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D16" s="11">
         <v>10</v>
@@ -3253,7 +3255,7 @@
         <v>9</v>
       </c>
       <c r="F16" s="11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G16" s="11">
         <v>8</v>
@@ -3271,49 +3273,49 @@
         <v>5</v>
       </c>
       <c r="L16" s="11">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M16" s="11">
         <v>3</v>
       </c>
       <c r="N16" s="11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O16" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P16" s="11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q16" s="11">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="R16" s="11">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="S16" s="11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T16" s="11">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="U16" s="11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V16" s="11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="W16" s="11">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X16" s="11">
         <v>2</v>
       </c>
       <c r="Y16" s="11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Z16" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -4026,11 +4028,11 @@
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" ref="C26:Z26" si="0">AVERAGE(C2:C7)+AVERAGE(C8:C13)*2+AVERAGE(C14:C19)*1.5+AVERAGE(C20:C25)*0.5</f>
-        <v>42.916666666666671</v>
+        <v>38.75</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>40.166666666666671</v>
+        <v>40.5</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
@@ -4038,87 +4040,87 @@
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>36.833333333333329</v>
+        <v>37.75</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>35.083333333333329</v>
+        <v>35.416666666666671</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
-        <v>32.666666666666664</v>
+        <v>33.5</v>
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>30.083333333333336</v>
+        <v>30.083333333333332</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>27.25</v>
+        <v>28.916666666666668</v>
       </c>
       <c r="K26">
         <f t="shared" si="0"/>
-        <v>25.916666666666664</v>
+        <v>25.749999999999996</v>
       </c>
       <c r="L26">
         <f t="shared" si="0"/>
-        <v>25.583333333333336</v>
+        <v>24.416666666666668</v>
       </c>
       <c r="M26">
         <f t="shared" si="0"/>
-        <v>25.083333333333332</v>
+        <v>25.916666666666664</v>
       </c>
       <c r="N26">
         <f t="shared" si="0"/>
-        <v>24.833333333333332</v>
+        <v>26.083333333333336</v>
       </c>
       <c r="O26">
         <f t="shared" si="0"/>
-        <v>24.75</v>
+        <v>23.5</v>
       </c>
       <c r="P26">
         <f t="shared" si="0"/>
-        <v>23.416666666666668</v>
+        <v>22.000000000000004</v>
       </c>
       <c r="Q26">
         <f t="shared" si="0"/>
-        <v>22.916666666666668</v>
+        <v>21.833333333333332</v>
       </c>
       <c r="R26">
         <f t="shared" si="0"/>
-        <v>22.833333333333332</v>
+        <v>21.333333333333332</v>
       </c>
       <c r="S26">
         <f t="shared" si="0"/>
-        <v>22.083333333333332</v>
+        <v>20.583333333333332</v>
       </c>
       <c r="T26">
         <f t="shared" si="0"/>
-        <v>21.166666666666668</v>
+        <v>19.750000000000004</v>
       </c>
       <c r="U26">
         <f t="shared" si="0"/>
-        <v>19.75</v>
+        <v>21</v>
       </c>
       <c r="V26">
         <f t="shared" si="0"/>
-        <v>18.666666666666668</v>
+        <v>16.833333333333332</v>
       </c>
       <c r="W26">
         <f t="shared" si="0"/>
-        <v>17.916666666666664</v>
+        <v>18.916666666666664</v>
       </c>
       <c r="X26">
         <f t="shared" si="0"/>
-        <v>17.333333333333332</v>
+        <v>18.333333333333332</v>
       </c>
       <c r="Y26">
         <f t="shared" si="0"/>
-        <v>17.166666666666668</v>
+        <v>16.333333333333332</v>
       </c>
       <c r="Z26">
         <f t="shared" si="0"/>
-        <v>16.666666666666668</v>
+        <v>17.083333333333336</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
@@ -4132,7 +4134,7 @@
       </c>
       <c r="C29">
         <f t="shared" ref="C29:Z29" si="1">AVERAGE(C2:C7)</f>
-        <v>5.666666666666667</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="D29">
         <f t="shared" si="1"/>
@@ -4148,15 +4150,15 @@
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>8.6666666666666661</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="H29">
         <f t="shared" si="1"/>
-        <v>4.833333333333333</v>
+        <v>5</v>
       </c>
       <c r="I29">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="J29">
         <f t="shared" si="1"/>
@@ -4164,19 +4166,19 @@
       </c>
       <c r="K29">
         <f t="shared" si="1"/>
-        <v>3.6666666666666665</v>
+        <v>3.5</v>
       </c>
       <c r="L29">
         <f t="shared" si="1"/>
-        <v>3.8333333333333335</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="M29">
         <f t="shared" si="1"/>
-        <v>5.5</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="N29">
         <f t="shared" si="1"/>
-        <v>4.333333333333333</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="O29">
         <f t="shared" si="1"/>
@@ -4196,7 +4198,7 @@
       </c>
       <c r="S29">
         <f t="shared" si="1"/>
-        <v>5.166666666666667</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="T29">
         <f t="shared" si="1"/>
@@ -4208,7 +4210,7 @@
       </c>
       <c r="V29">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="W29">
         <f t="shared" si="1"/>
@@ -4216,11 +4218,11 @@
       </c>
       <c r="X29">
         <f t="shared" si="1"/>
-        <v>5.833333333333333</v>
+        <v>6.166666666666667</v>
       </c>
       <c r="Y29">
         <f t="shared" si="1"/>
-        <v>6.166666666666667</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="Z29">
         <f t="shared" si="1"/>
@@ -4233,11 +4235,11 @@
       </c>
       <c r="C30">
         <f t="shared" ref="C30:Z30" si="2">AVERAGE(C8:C13)</f>
-        <v>10</v>
+        <v>8.6666666666666661</v>
       </c>
       <c r="D30">
         <f t="shared" si="2"/>
-        <v>9.8333333333333339</v>
+        <v>10</v>
       </c>
       <c r="E30">
         <f t="shared" si="2"/>
@@ -4245,23 +4247,23 @@
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="G30">
         <f t="shared" si="2"/>
-        <v>5.333333333333333</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>6.833333333333333</v>
       </c>
       <c r="I30">
         <f t="shared" si="2"/>
-        <v>4.166666666666667</v>
+        <v>4</v>
       </c>
       <c r="J30">
         <f t="shared" si="2"/>
-        <v>4.166666666666667</v>
+        <v>5</v>
       </c>
       <c r="K30">
         <f t="shared" si="2"/>
@@ -4277,19 +4279,19 @@
       </c>
       <c r="N30">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>3.8333333333333335</v>
       </c>
       <c r="O30">
         <f t="shared" si="2"/>
-        <v>5.666666666666667</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="P30">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="Q30">
         <f t="shared" si="2"/>
-        <v>4.666666666666667</v>
+        <v>4.5</v>
       </c>
       <c r="R30">
         <f t="shared" si="2"/>
@@ -4297,19 +4299,19 @@
       </c>
       <c r="S30">
         <f t="shared" si="2"/>
-        <v>5.333333333333333</v>
+        <v>5</v>
       </c>
       <c r="T30">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="U30">
         <f t="shared" si="2"/>
-        <v>2.6666666666666665</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="V30">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="W30">
         <f t="shared" si="2"/>
@@ -4317,7 +4319,7 @@
       </c>
       <c r="X30">
         <f t="shared" si="2"/>
-        <v>3.8333333333333335</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="Y30">
         <f t="shared" si="2"/>
@@ -4325,7 +4327,7 @@
       </c>
       <c r="Z30">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>2.3333333333333335</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
@@ -4334,7 +4336,7 @@
       </c>
       <c r="C31">
         <f t="shared" ref="C31:Z31" si="3">AVERAGE(C14:C19)</f>
-        <v>9.8333333333333339</v>
+        <v>9.5</v>
       </c>
       <c r="D31">
         <f t="shared" si="3"/>
@@ -4346,7 +4348,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="3"/>
-        <v>9.6666666666666661</v>
+        <v>9.8333333333333339</v>
       </c>
       <c r="G31">
         <f t="shared" si="3"/>
@@ -4370,7 +4372,7 @@
       </c>
       <c r="L31">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="M31">
         <f t="shared" si="3"/>
@@ -4378,43 +4380,43 @@
       </c>
       <c r="N31">
         <f t="shared" si="3"/>
-        <v>7.666666666666667</v>
+        <v>7.833333333333333</v>
       </c>
       <c r="O31">
         <f t="shared" si="3"/>
-        <v>5.333333333333333</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="P31">
         <f t="shared" si="3"/>
-        <v>8.1666666666666661</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="Q31">
         <f t="shared" si="3"/>
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="R31">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S31">
         <f t="shared" si="3"/>
-        <v>2.5</v>
+        <v>2.1666666666666665</v>
       </c>
       <c r="T31">
         <f t="shared" si="3"/>
-        <v>6.666666666666667</v>
+        <v>6.166666666666667</v>
       </c>
       <c r="U31">
         <f t="shared" si="3"/>
-        <v>5.166666666666667</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="V31">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="W31">
         <f t="shared" si="3"/>
-        <v>5.5</v>
+        <v>6.166666666666667</v>
       </c>
       <c r="X31">
         <f t="shared" si="3"/>
@@ -4422,11 +4424,11 @@
       </c>
       <c r="Y31">
         <f t="shared" si="3"/>
-        <v>3.5</v>
+        <v>2.8333333333333335</v>
       </c>
       <c r="Z31">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3.8333333333333335</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>